<commit_message>
file dooring dan haulage untuk data berat dan jarak trucking
</commit_message>
<xml_diff>
--- a/Hasil_Analisa_Regresi_Unit_Fix.xlsx
+++ b/Hasil_Analisa_Regresi_Unit_Fix.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Downloads\SPIL\bbm\Analisa BBM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7F280CC-64A7-4097-B2E6-A606BF82CFE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AF20781-30A4-4E60-8229-1F93F7B1C748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -852,8 +852,8 @@
   <dimension ref="A1:G180"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
+      <pane ySplit="1" topLeftCell="A155" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -861,9 +861,9 @@
     <col min="1" max="1" width="30" customWidth="1"/>
     <col min="2" max="2" width="15.42578125" customWidth="1"/>
     <col min="3" max="3" width="22.140625" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" customWidth="1"/>
-    <col min="5" max="5" width="24.140625" customWidth="1"/>
-    <col min="6" max="6" width="22" customWidth="1"/>
+    <col min="4" max="4" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>